<commit_message>
Update tasks with new ideas
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -127,6 +127,51 @@
   </si>
   <si>
     <t>Wand of Magic Missiles -&gt; depends on Magic Missile</t>
+  </si>
+  <si>
+    <t>Mob Item Slots</t>
+  </si>
+  <si>
+    <t>Mob Gear Armor and Shields</t>
+  </si>
+  <si>
+    <t>Armor Type</t>
+  </si>
+  <si>
+    <t>Weapon Attack Adjustments</t>
+  </si>
+  <si>
+    <t>Potion - Healing - various</t>
+  </si>
+  <si>
+    <t>Potion - Heroism</t>
+  </si>
+  <si>
+    <t>Potion - Invisibility</t>
+  </si>
+  <si>
+    <t>Potion - Invulnerability</t>
+  </si>
+  <si>
+    <t>Scroll - summoning</t>
+  </si>
+  <si>
+    <t>Scroll - protection</t>
+  </si>
+  <si>
+    <t>Ring - Free Action</t>
+  </si>
+  <si>
+    <t>Ring - Fire Resistance</t>
+  </si>
+  <si>
+    <t>Ring - Protection</t>
+  </si>
+  <si>
+    <t>Cloak of Displacement</t>
+  </si>
+  <si>
+    <t>Post Combat Cleanup.  Flags, reset once per combat</t>
   </si>
 </sst>
 </file>
@@ -465,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,201 +575,276 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>100</v>
-      </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>101</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>101</v>
-      </c>
       <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>110</v>
-      </c>
       <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>111</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14">
-        <v>110</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>110</v>
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>120</v>
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
         <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>120</v>
       </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D23">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24">
+        <v>124</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>130</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>120</v>
+      </c>
+      <c r="E26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>131</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>132</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" t="s">
         <v>23</v>
       </c>
-      <c r="D24">
+      <c r="D28">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29">
         <v>133</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" t="s">
         <v>21</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mob special att/de & Magic Resistance
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Task</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>Post Combat Cleanup.  Flags, reset once per combat</t>
+  </si>
+  <si>
+    <t>Mob Special Attack/Defense, Magic Resistance</t>
   </si>
 </sst>
 </file>
@@ -510,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H49"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,56 +603,50 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <v>100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>101</v>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
         <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>110</v>
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>110</v>
@@ -657,32 +654,32 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21">
-        <v>120</v>
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>120</v>
@@ -690,10 +687,10 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23">
         <v>120</v>
@@ -701,46 +698,46 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24">
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>130</v>
-      </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>124</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25">
         <v>120</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D27">
-        <v>130</v>
+        <v>120</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D28">
         <v>130</v>
@@ -748,102 +745,113 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D29">
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>5</v>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>133</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add return to exit before extraneous code
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Multiple Battles In BattleGroup Resolving Simultaneously</t>
+  </si>
+  <si>
+    <t>Master Game Loop</t>
   </si>
 </sst>
 </file>
@@ -648,6 +651,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>90</v>
@@ -656,7 +670,7 @@
         <v>54</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>91</v>

</xml_diff>

<commit_message>
Rename Person.js to Mob.js
Test fixed to use new name.
all tests pass as of now.
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Master Game Loop</t>
+  </si>
+  <si>
+    <t>Add Dwarf. Note ac bonus vs giants</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="B2:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,6 +652,14 @@
       </c>
       <c r="D14">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>